<commit_message>
BackLog primo secondo e terzo sprint
</commit_message>
<xml_diff>
--- a/BackLog.xlsx
+++ b/BackLog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="40">
   <si>
     <t xml:space="preserve">Task name</t>
   </si>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">produzione diagramma delle classi </t>
   </si>
   <si>
-    <t xml:space="preserve">Sprint 2 (Programmazione)</t>
+    <t xml:space="preserve">Sprint 2</t>
   </si>
   <si>
     <t xml:space="preserve">messa a termine del diagramma dei casi d’uso</t>
@@ -116,6 +116,30 @@
   </si>
   <si>
     <t xml:space="preserve">Rossi, Corradi, Zheng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 3 (Programmazione)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creazione classe Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To do</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creazione metodo Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creazione metodo Registrazione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rossi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creazione classe Passeggero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correzione diagramma delle classi</t>
   </si>
 </sst>
 </file>
@@ -307,10 +331,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -543,6 +567,101 @@
         <v>31</v>
       </c>
     </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>